<commit_message>
Redefine CDM max as 1
</commit_message>
<xml_diff>
--- a/Example implementation/Excel usage example.xlsx
+++ b/Example implementation/Excel usage example.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shannon\Documents\0Schoolwork\Cubicity metric paper\CDMdata\Example implementation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89445D80-818B-460B-A86E-9FF7D7AD1BC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{489C4E47-8BB2-4784-A603-F3C96F3D4ADF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13290" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -433,7 +433,7 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="P22" sqref="P22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -487,8 +487,8 @@
         <v>63</v>
       </c>
       <c r="G2">
-        <f>SUM(ROUND(ABS(C2/SQRT(B2^2+C2^2-2*C2*B2*ROUND(COS(IF(D2&lt;90,RADIANS(180-D2),RADIANS(D2))),4))-1/SQRT(2)),4),ROUND(ABS(B2/SQRT(C2^2+B2^2-2*B2*C2*ROUND(COS(IF(D2&lt;90,RADIANS(180-D2),RADIANS(D2))),4))-1/SQRT(2)),4),ROUND(ABS(C2/SQRT(A2^2+C2^2-2*C2*A2*ROUND(COS(IF(E2&lt;90,RADIANS(180-E2),RADIANS(E2))),4))-1/SQRT(2)),4),ROUND(ABS(A2/SQRT(C2^2+A2^2-2*A2*C2*ROUND(COS(IF(E2&lt;90,RADIANS(180-E2),RADIANS(E2))),4))-1/SQRT(2)),4),ROUND(ABS(A2/SQRT(A2^2+B2^2-2*A2*B2*ROUND(COS(IF(F2&lt;90,RADIANS(180-F2),RADIANS(F2))),4))-1/SQRT(2)),4),ROUND(ABS(B2/SQRT(A2^2+B2^2-2*A2*B2*ROUND(COS(IF(F2&lt;90,RADIANS(180-F2),RADIANS(F2))),4))-1/SQRT(2)),4))</f>
-        <v>1.2029000000000001</v>
+        <f>SUM(ROUND(ABS(C2/SQRT(B2^2+C2^2-2*C2*B2*ROUND(COS(IF(D2&lt;90,RADIANS(180-D2),RADIANS(D2))),4))-1/SQRT(2)),4),ROUND(ABS(B2/SQRT(C2^2+B2^2-2*B2*C2*ROUND(COS(IF(D2&lt;90,RADIANS(180-D2),RADIANS(D2))),4))-1/SQRT(2)),4),ROUND(ABS(C2/SQRT(A2^2+C2^2-2*C2*A2*ROUND(COS(IF(E2&lt;90,RADIANS(180-E2),RADIANS(E2))),4))-1/SQRT(2)),4),ROUND(ABS(A2/SQRT(C2^2+A2^2-2*A2*C2*ROUND(COS(IF(E2&lt;90,RADIANS(180-E2),RADIANS(E2))),4))-1/SQRT(2)),4),ROUND(ABS(A2/SQRT(A2^2+B2^2-2*A2*B2*ROUND(COS(IF(F2&lt;90,RADIANS(180-F2),RADIANS(F2))),4))-1/SQRT(2)),4),ROUND(ABS(B2/SQRT(A2^2+B2^2-2*A2*B2*ROUND(COS(IF(F2&lt;90,RADIANS(180-F2),RADIANS(F2))),4))-1/SQRT(2)),4))/3</f>
+        <v>0.40096666666666669</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -511,8 +511,8 @@
         <v>63</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="G3:G11" si="0">SUM(ROUND(ABS(C3/SQRT(B3^2+C3^2-2*C3*B3*ROUND(COS(IF(D3&lt;90,RADIANS(180-D3),RADIANS(D3))),4))-1/SQRT(2)),4),ROUND(ABS(B3/SQRT(C3^2+B3^2-2*B3*C3*ROUND(COS(IF(D3&lt;90,RADIANS(180-D3),RADIANS(D3))),4))-1/SQRT(2)),4))</f>
-        <v>0.40179999999999999</v>
+        <f t="shared" ref="G3:G11" si="0">SUM(ROUND(ABS(C3/SQRT(B3^2+C3^2-2*C3*B3*ROUND(COS(IF(D3&lt;90,RADIANS(180-D3),RADIANS(D3))),4))-1/SQRT(2)),4),ROUND(ABS(B3/SQRT(C3^2+B3^2-2*B3*C3*ROUND(COS(IF(D3&lt;90,RADIANS(180-D3),RADIANS(D3))),4))-1/SQRT(2)),4),ROUND(ABS(C3/SQRT(A3^2+C3^2-2*C3*A3*ROUND(COS(IF(E3&lt;90,RADIANS(180-E3),RADIANS(E3))),4))-1/SQRT(2)),4),ROUND(ABS(A3/SQRT(C3^2+A3^2-2*A3*C3*ROUND(COS(IF(E3&lt;90,RADIANS(180-E3),RADIANS(E3))),4))-1/SQRT(2)),4),ROUND(ABS(A3/SQRT(A3^2+B3^2-2*A3*B3*ROUND(COS(IF(F3&lt;90,RADIANS(180-F3),RADIANS(F3))),4))-1/SQRT(2)),4),ROUND(ABS(B3/SQRT(A3^2+B3^2-2*A3*B3*ROUND(COS(IF(F3&lt;90,RADIANS(180-F3),RADIANS(F3))),4))-1/SQRT(2)),4))/3</f>
+        <v>0.58043333333333347</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -536,7 +536,7 @@
       </c>
       <c r="G4">
         <f t="shared" si="0"/>
-        <v>0.44720000000000004</v>
+        <v>0.29813333333333336</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -584,7 +584,7 @@
       </c>
       <c r="G6">
         <f t="shared" si="0"/>
-        <v>0.34889999999999999</v>
+        <v>0.23393333333333333</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -608,7 +608,7 @@
       </c>
       <c r="G7">
         <f t="shared" si="0"/>
-        <v>0.27980000000000005</v>
+        <v>0.21346666666666669</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -632,7 +632,7 @@
       </c>
       <c r="G8">
         <f t="shared" si="0"/>
-        <v>0.38590000000000002</v>
+        <v>0.34966666666666663</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -656,7 +656,7 @@
       </c>
       <c r="G9">
         <f t="shared" si="0"/>
-        <v>0.28570000000000001</v>
+        <v>0.20956666666666668</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -680,7 +680,7 @@
       </c>
       <c r="G10">
         <f t="shared" si="0"/>
-        <v>0.1119</v>
+        <v>0.24206666666666665</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -704,7 +704,7 @@
       </c>
       <c r="G11">
         <f t="shared" si="0"/>
-        <v>0.2112</v>
+        <v>0.22973333333333334</v>
       </c>
     </row>
   </sheetData>

</xml_diff>